<commit_message>
Add parts to inventory
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DEB4D5-7DDF-406C-B649-6BFD17A218E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2397A735-97E6-45FA-9D7B-FEC2F181AA94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17620" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="3170" yWindow="1860" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -208,6 +208,207 @@
   </si>
   <si>
     <t>Assembled 2x microstrip-test-4-layer-sma-v1</t>
+  </si>
+  <si>
+    <t>Coilcraft</t>
+  </si>
+  <si>
+    <t>0402CS-1N8XGL</t>
+  </si>
+  <si>
+    <t>0402 inductor, 1.8n</t>
+  </si>
+  <si>
+    <t>994-0402CS-1N8XGLU</t>
+  </si>
+  <si>
+    <t>0402HP-18NXGL</t>
+  </si>
+  <si>
+    <t>0402 inductor, 18n</t>
+  </si>
+  <si>
+    <t>994-0402HP-18NXGLU</t>
+  </si>
+  <si>
+    <t>0402CS-2N0XGL</t>
+  </si>
+  <si>
+    <t>0402 inductor, 2.0n</t>
+  </si>
+  <si>
+    <t>994-0402CS-2N0XGLW</t>
+  </si>
+  <si>
+    <t>0402HP-47NXGL</t>
+  </si>
+  <si>
+    <t>0402 inductor, 47n</t>
+  </si>
+  <si>
+    <t>994-0402HP-47NXGLU</t>
+  </si>
+  <si>
+    <t>MPD</t>
+  </si>
+  <si>
+    <t>SBH431-1AS</t>
+  </si>
+  <si>
+    <t>3x AAA battery holder, cover, 6" leads, switch</t>
+  </si>
+  <si>
+    <t>SBH431-1AS-ND</t>
+  </si>
+  <si>
+    <t>Harwin</t>
+  </si>
+  <si>
+    <t>M20-9994045</t>
+  </si>
+  <si>
+    <t>952-3307-ND</t>
+  </si>
+  <si>
+    <t>M20-1060200</t>
+  </si>
+  <si>
+    <t>2.54mm housing, 2 position</t>
+  </si>
+  <si>
+    <t>952-2227-ND</t>
+  </si>
+  <si>
+    <t>M20-1160042</t>
+  </si>
+  <si>
+    <t>Socket contact, gold, crimp, 22-30 AWG</t>
+  </si>
+  <si>
+    <t>952-2157-1-ND</t>
+  </si>
+  <si>
+    <t>M20-1060400</t>
+  </si>
+  <si>
+    <t>2.54mm housing, 4 position</t>
+  </si>
+  <si>
+    <t>952-2229-ND</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00‎</t>
+  </si>
+  <si>
+    <t>0603 resistor, 0, jumper</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00CT-ND‎</t>
+  </si>
+  <si>
+    <t>RMCF0603FT2K70‎</t>
+  </si>
+  <si>
+    <t>0603 resistor, 2.7k, 1%, 100ppm</t>
+  </si>
+  <si>
+    <t>RMCF0603FT2K70CT-ND‎</t>
+  </si>
+  <si>
+    <t>RMCF0402FT47K0‎</t>
+  </si>
+  <si>
+    <t>0402 resistor, 47k, 1%, 100ppm</t>
+  </si>
+  <si>
+    <t>‎RMCF0402FT47K0CT-ND‎</t>
+  </si>
+  <si>
+    <t>RMCF0402ZT0R00‎</t>
+  </si>
+  <si>
+    <t>0402 resistor, 0, jumper</t>
+  </si>
+  <si>
+    <t>RMCF0402ZT0R00CT-ND‎</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>LP38692MP-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulator, 1A, EN, 3.3V Fixed</t>
+  </si>
+  <si>
+    <t>LP38692MP-3.3/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>2.54mm header, vertical strip, 1x40</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>CL10A105KA8NNNC</t>
+  </si>
+  <si>
+    <t>0603 capacitor, 1u, X5R, 25V</t>
+  </si>
+  <si>
+    <t>1276-1102-1-ND</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNG</t>
+  </si>
+  <si>
+    <t>0805 capactior, 10u, X5R, 16V</t>
+  </si>
+  <si>
+    <t>1276-6455-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B223KA8NNNC</t>
+  </si>
+  <si>
+    <t>0603 capacitor, 22n, X7R, 25V</t>
+  </si>
+  <si>
+    <t>1276-1999-1-ND</t>
+  </si>
+  <si>
+    <t>CL05C561JB5NNNC</t>
+  </si>
+  <si>
+    <t>0402 capacitor, 560p, C0G, 50V</t>
+  </si>
+  <si>
+    <t>1276-1709-1-ND</t>
+  </si>
+  <si>
+    <t>ROHM Semi.</t>
+  </si>
+  <si>
+    <t>SML-D13M8WT86</t>
+  </si>
+  <si>
+    <t>0603 LED, GREEN, Diffused</t>
+  </si>
+  <si>
+    <t>‎846-1198-1-ND‎</t>
+  </si>
+  <si>
+    <t>SML-D12U8WT86‎</t>
+  </si>
+  <si>
+    <t>0603 LED, RED, Diffused</t>
+  </si>
+  <si>
+    <t>511-1580-1-ND‎</t>
   </si>
 </sst>
 </file>
@@ -271,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -300,6 +501,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C355E92D-4F29-4448-8517-BC8F08AC5F2B}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -629,8 +833,8 @@
     <col min="4" max="4" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
-    <col min="8" max="8" width="40.36328125" customWidth="1"/>
+    <col min="7" max="7" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13">
@@ -945,103 +1149,563 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="A21" s="2">
+        <v>2</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="25" spans="1:8" ht="13">
-      <c r="A25" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="A22" s="2">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2">
+        <v>25</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2">
+        <v>100</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2">
+        <v>100</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
+      <c r="A27" s="2">
+        <v>100</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2">
-        <v>1</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2">
+        <v>25</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2">
+        <v>100</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="2">
+        <v>100</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="2">
+        <v>100</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="2">
+        <v>100</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" t="s">
+        <v>116</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>117</v>
+      </c>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="2">
+        <v>10</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
+        <v>121</v>
+      </c>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="2">
+        <v>10</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>124</v>
+      </c>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="B37" s="8"/>
+      <c r="C37" s="13"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" s="8"/>
+      <c r="C38" s="13"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="8"/>
+      <c r="C39" s="13"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40" s="8"/>
+      <c r="C40" s="13"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41" s="8"/>
+      <c r="C41" s="13"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="45" spans="1:8" ht="13">
+      <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="2">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
         <v>2</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B49" s="12">
         <v>43675</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C49" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H22" xr:uid="{12ABAAD2-10AD-445B-A38F-77CAAD4446E7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H22">
-      <sortCondition ref="C5:C22"/>
-      <sortCondition ref="D5:D22"/>
+  <autoFilter ref="A4:H42" xr:uid="{12ABAAD2-10AD-445B-A38F-77CAAD4446E7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H42">
+      <sortCondition ref="C5:C42"/>
+      <sortCondition ref="D5:D42"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Assembled 1x dual-synthesizer board
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2397A735-97E6-45FA-9D7B-FEC2F181AA94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA1A347-9E81-48B9-82AE-2B287997F793}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3170" yWindow="1860" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="20140" yWindow="9330" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="126">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -102,9 +102,6 @@
     <t>BGB707L7ESDE6327XTSA1</t>
   </si>
   <si>
-    <t>General RF LNA, very low input</t>
-  </si>
-  <si>
     <t>726-SP000531308</t>
   </si>
   <si>
@@ -120,27 +117,15 @@
     <t>BDCN-20-13+</t>
   </si>
   <si>
-    <t>Bi-directional coupler</t>
-  </si>
-  <si>
     <t>BPF-C450+</t>
   </si>
   <si>
-    <t>BPF, 400 - 510 MHz</t>
-  </si>
-  <si>
     <t>BPF-F1250</t>
   </si>
   <si>
-    <t>BPF, 1050 - 1450 MHz</t>
-  </si>
-  <si>
     <t>MAC-24+</t>
   </si>
   <si>
-    <t>Diode Ring Mixer</t>
-  </si>
-  <si>
     <t>QCN-19+</t>
   </si>
   <si>
@@ -153,9 +138,6 @@
     <t>856930</t>
   </si>
   <si>
-    <t>457.5 MHz SAW, 15 MHz</t>
-  </si>
-  <si>
     <t>772-856930</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>TQP3M9036</t>
   </si>
   <si>
-    <t>RF LNA, 0.4 - 2.0 GHz</t>
-  </si>
-  <si>
     <t>772-TQP3M9036</t>
   </si>
   <si>
@@ -216,36 +195,24 @@
     <t>0402CS-1N8XGL</t>
   </si>
   <si>
-    <t>0402 inductor, 1.8n</t>
-  </si>
-  <si>
     <t>994-0402CS-1N8XGLU</t>
   </si>
   <si>
     <t>0402HP-18NXGL</t>
   </si>
   <si>
-    <t>0402 inductor, 18n</t>
-  </si>
-  <si>
     <t>994-0402HP-18NXGLU</t>
   </si>
   <si>
     <t>0402CS-2N0XGL</t>
   </si>
   <si>
-    <t>0402 inductor, 2.0n</t>
-  </si>
-  <si>
     <t>994-0402CS-2N0XGLW</t>
   </si>
   <si>
     <t>0402HP-47NXGL</t>
   </si>
   <si>
-    <t>0402 inductor, 47n</t>
-  </si>
-  <si>
     <t>994-0402HP-47NXGLU</t>
   </si>
   <si>
@@ -255,9 +222,6 @@
     <t>SBH431-1AS</t>
   </si>
   <si>
-    <t>3x AAA battery holder, cover, 6" leads, switch</t>
-  </si>
-  <si>
     <t>SBH431-1AS-ND</t>
   </si>
   <si>
@@ -303,36 +267,24 @@
     <t>RMCF0603ZT0R00‎</t>
   </si>
   <si>
-    <t>0603 resistor, 0, jumper</t>
-  </si>
-  <si>
     <t>RMCF0603ZT0R00CT-ND‎</t>
   </si>
   <si>
     <t>RMCF0603FT2K70‎</t>
   </si>
   <si>
-    <t>0603 resistor, 2.7k, 1%, 100ppm</t>
-  </si>
-  <si>
     <t>RMCF0603FT2K70CT-ND‎</t>
   </si>
   <si>
     <t>RMCF0402FT47K0‎</t>
   </si>
   <si>
-    <t>0402 resistor, 47k, 1%, 100ppm</t>
-  </si>
-  <si>
     <t>‎RMCF0402FT47K0CT-ND‎</t>
   </si>
   <si>
     <t>RMCF0402ZT0R00‎</t>
   </si>
   <si>
-    <t>0402 resistor, 0, jumper</t>
-  </si>
-  <si>
     <t>RMCF0402ZT0R00CT-ND‎</t>
   </si>
   <si>
@@ -348,45 +300,30 @@
     <t>LP38692MP-3.3/NOPBCT-ND</t>
   </si>
   <si>
-    <t>2.54mm header, vertical strip, 1x40</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
     <t>CL10A105KA8NNNC</t>
   </si>
   <si>
-    <t>0603 capacitor, 1u, X5R, 25V</t>
-  </si>
-  <si>
     <t>1276-1102-1-ND</t>
   </si>
   <si>
     <t>CL21A106KOQNNNG</t>
   </si>
   <si>
-    <t>0805 capactior, 10u, X5R, 16V</t>
-  </si>
-  <si>
     <t>1276-6455-1-ND</t>
   </si>
   <si>
     <t>CL10B223KA8NNNC</t>
   </si>
   <si>
-    <t>0603 capacitor, 22n, X7R, 25V</t>
-  </si>
-  <si>
     <t>1276-1999-1-ND</t>
   </si>
   <si>
     <t>CL05C561JB5NNNC</t>
   </si>
   <si>
-    <t>0402 capacitor, 560p, C0G, 50V</t>
-  </si>
-  <si>
     <t>1276-1709-1-ND</t>
   </si>
   <si>
@@ -396,19 +333,85 @@
     <t>SML-D13M8WT86</t>
   </si>
   <si>
-    <t>0603 LED, GREEN, Diffused</t>
-  </si>
-  <si>
     <t>‎846-1198-1-ND‎</t>
   </si>
   <si>
     <t>SML-D12U8WT86‎</t>
   </si>
   <si>
-    <t>0603 LED, RED, Diffused</t>
-  </si>
-  <si>
     <t>511-1580-1-ND‎</t>
+  </si>
+  <si>
+    <t>Assembled 1x dual-synthesizer</t>
+  </si>
+  <si>
+    <t>2.54mm header, vertical strip, 1x40 (by x1)</t>
+  </si>
+  <si>
+    <t>C - 0603, 1u, X5R, 25V</t>
+  </si>
+  <si>
+    <t>C - 0603, 22n, X7R, 25V</t>
+  </si>
+  <si>
+    <t>C - 0402, 560p, C0G, 50V</t>
+  </si>
+  <si>
+    <t>R - 0402, 0, jumper</t>
+  </si>
+  <si>
+    <t>R - 0402, 47k, 1%, 100ppm</t>
+  </si>
+  <si>
+    <t>R - 0603, 0, jumper</t>
+  </si>
+  <si>
+    <t>R - 0603, 2.7k, 1%, 100ppm</t>
+  </si>
+  <si>
+    <t>L - 0402, 1.8n</t>
+  </si>
+  <si>
+    <t>L - 0402, 18n</t>
+  </si>
+  <si>
+    <t>L - 0402, 2.0n</t>
+  </si>
+  <si>
+    <t>L - 0402, 47n</t>
+  </si>
+  <si>
+    <t>LED - 0603, GREEN, Diffused</t>
+  </si>
+  <si>
+    <t>LED - 0603, RED, Diffused</t>
+  </si>
+  <si>
+    <t>C - 0805, 10u, X5R, 16V</t>
+  </si>
+  <si>
+    <t>Battery holder, 3x AAA, cover, 6" leads, switch</t>
+  </si>
+  <si>
+    <t>Filter - SAW, 457.5 MHz, 15 MHz</t>
+  </si>
+  <si>
+    <t>Filter - BPF, 1050 - 1450 MHz</t>
+  </si>
+  <si>
+    <t>Filter - BPF, 400 - 510 MHz</t>
+  </si>
+  <si>
+    <t>Mixer - double balanced</t>
+  </si>
+  <si>
+    <t>LNA, general, very low input</t>
+  </si>
+  <si>
+    <t>LNA, 0.4 - 2.0 GHz</t>
+  </si>
+  <si>
+    <t>Coupler - Bi-directional</t>
   </si>
 </sst>
 </file>
@@ -819,10 +822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C355E92D-4F29-4448-8517-BC8F08AC5F2B}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -870,377 +874,381 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="C5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>14</v>
+      <c r="G5" t="s">
+        <v>65</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>19</v>
+      <c r="C6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>23</v>
+      <c r="C7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="6"/>
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="6"/>
+      <c r="C9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="6"/>
+      <c r="C10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>90</v>
+      </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>99</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="E13" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -1252,379 +1260,375 @@
         <v>9</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
-        <v>83</v>
+      <c r="C24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
-        <v>86</v>
+      <c r="C25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>90</v>
-      </c>
+      <c r="C26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>93</v>
+      <c r="C27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" t="s">
-        <v>96</v>
+      <c r="C28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="2">
+      <c r="A29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" t="s">
-        <v>99</v>
-      </c>
+      <c r="D29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" t="s">
         <v>109</v>
-      </c>
-      <c r="E32" t="s">
-        <v>110</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" t="s">
-        <v>116</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="C34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G34" t="s">
-        <v>117</v>
+      <c r="G34" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" t="s">
-        <v>123</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>124</v>
+      <c r="C36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="H36" s="6"/>
     </row>
@@ -1654,58 +1658,128 @@
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="45" spans="1:8" ht="13">
-      <c r="A45" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="13"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="B43" s="8"/>
+      <c r="C43" s="13"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" s="8"/>
+      <c r="C44" s="13"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="B45" s="8"/>
+      <c r="C45" s="13"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46" s="8"/>
+      <c r="C46" s="13"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="13"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" s="8"/>
+      <c r="C48" s="13"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="B49" s="8"/>
+      <c r="C49" s="13"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="B50" s="8"/>
+      <c r="C50" s="13"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="B51" s="8"/>
+      <c r="C51" s="13"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="8"/>
+      <c r="C52" s="13"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="B53" s="8"/>
+      <c r="C53" s="13"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="9"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+    </row>
+    <row r="57" spans="1:8" ht="13">
+      <c r="A57" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="2">
+    <row r="60" spans="1:8">
+      <c r="A60" s="2">
         <v>1</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="2">
+      <c r="B60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="2">
         <v>2</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B61" s="12">
         <v>43675</v>
       </c>
-      <c r="C49" t="s">
-        <v>57</v>
+      <c r="C61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="2">
+        <v>3</v>
+      </c>
+      <c r="B62" s="12">
+        <v>43700</v>
+      </c>
+      <c r="C62" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H42" xr:uid="{12ABAAD2-10AD-445B-A38F-77CAAD4446E7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H42">
-      <sortCondition ref="C5:C42"/>
-      <sortCondition ref="D5:D42"/>
+  <autoFilter ref="A4:H54" xr:uid="{12ABAAD2-10AD-445B-A38F-77CAAD4446E7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H54">
+      <sortCondition ref="E4:E54"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add boards inventory sheet
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA1A347-9E81-48B9-82AE-2B287997F793}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F52611E-685A-46CD-B7C7-22D73C16A5FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20140" yWindow="9330" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="-11200" yWindow="4580" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Boards" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$54</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="142">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -412,6 +413,54 @@
   </si>
   <si>
     <t>Coupler - Bi-directional</t>
+  </si>
+  <si>
+    <t>Inventory of evaluation boards</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Assembled</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>amp-LNA-L-band-TQP3M9037</t>
+  </si>
+  <si>
+    <t>amp-LNA-S-band-TQP3M9037</t>
+  </si>
+  <si>
+    <t>amp-LNA-UHF-TQP3M9036</t>
+  </si>
+  <si>
+    <t>bpf-IF-SAW-856930</t>
+  </si>
+  <si>
+    <t>mixer-MAC-24+</t>
+  </si>
+  <si>
+    <t>power-linear-LP38692</t>
+  </si>
+  <si>
+    <t>power-switching-TPS6211x</t>
+  </si>
+  <si>
+    <t>synthesizer-RF-Si4123</t>
+  </si>
+  <si>
+    <t>microstrip-test-4-layer-sma-v1</t>
+  </si>
+  <si>
+    <t>RCVD</t>
+  </si>
+  <si>
+    <t>PEND</t>
+  </si>
+  <si>
+    <t>ORD ?</t>
   </si>
 </sst>
 </file>
@@ -475,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -507,6 +556,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,7 +881,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1785,4 +1840,136 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7200ED79-E8BF-4B26-BED8-4868A9C7408E}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A20" sqref="A19:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="30.08984375" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" customWidth="1"/>
+    <col min="3" max="4" width="10.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.36328125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="14"/>
+    </row>
+    <row r="5" spans="1:5" ht="13">
+      <c r="A5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:E14">
+    <sortCondition ref="A5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Received Qorvo LNA boards
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F52611E-685A-46CD-B7C7-22D73C16A5FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88995AFC-A434-4B07-B8B8-450FAD2884B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11200" yWindow="4580" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="5170" yWindow="1460" windowWidth="23190" windowHeight="14770" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -458,9 +458,6 @@
   </si>
   <si>
     <t>PEND</t>
-  </si>
-  <si>
-    <t>ORD ?</t>
   </si>
 </sst>
 </file>
@@ -881,7 +878,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1847,7 +1844,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A19:A20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1885,24 +1882,33 @@
       <c r="A6" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>141</v>
+      <c r="B6" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>141</v>
+      <c r="B7" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>141</v>
+      <c r="B8" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5">

</xml_diff>

<commit_message>
Inventory, add stencils column for boards
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2696F46-8E4A-426A-8237-2F74EB9C4A3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4015DD-4514-436E-8348-C437345C23C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17620" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="25360" yWindow="2990" windowWidth="13240" windowHeight="14170" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Boards" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boards!$A$5:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boards!$A$5:$F$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="148">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -474,6 +474,12 @@
   </si>
   <si>
     <t>synthesizer-IF-Si4112</t>
+  </si>
+  <si>
+    <t>Stencil</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -894,7 +900,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1876,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7200ED79-E8BF-4B26-BED8-4868A9C7408E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1887,16 +1893,17 @@
     <col min="1" max="1" width="30.08984375" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="4" width="10.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.36328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="5" spans="1:5" ht="13">
+    <row r="5" spans="1:6" ht="13">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
@@ -1910,10 +1917,13 @@
         <v>128</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -1923,8 +1933,11 @@
       <c r="C6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -1934,8 +1947,11 @@
       <c r="C7" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -1945,16 +1961,22 @@
       <c r="C8" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>133</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -1967,40 +1989,55 @@
       <c r="D10" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>134</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>135</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>136</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -2013,14 +2050,17 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
+      <c r="E15" s="15" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:E15" xr:uid="{50C1A60C-E47A-486F-B8CF-18CEB4A5343D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:E15">
+  <autoFilter ref="A5:F15" xr:uid="{50C1A60C-E47A-486F-B8CF-18CEB4A5343D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F15">
       <sortCondition ref="A5:A15"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:E14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F14">
     <sortCondition ref="A5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Board inventory, ordered some boards and stencils
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4015DD-4514-436E-8348-C437345C23C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74405AC2-D3B3-4F23-BCDC-AF28A8DF1510}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25360" yWindow="2990" windowWidth="13240" windowHeight="14170" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="14630" yWindow="1420" windowWidth="16320" windowHeight="16020" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <t>RCVD</t>
   </si>
   <si>
-    <t>PEND</t>
-  </si>
-  <si>
     <t>AX5043-1-TW30</t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>ORDR</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -580,6 +580,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -898,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C355E92D-4F29-4448-8517-BC8F08AC5F2B}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1642,19 +1645,19 @@
         <v>9</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H34" s="6"/>
     </row>
@@ -1884,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7200ED79-E8BF-4B26-BED8-4868A9C7408E}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1917,7 +1920,7 @@
         <v>128</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -1933,8 +1936,8 @@
       <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>140</v>
+      <c r="E6" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1947,8 +1950,8 @@
       <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>140</v>
+      <c r="E7" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1961,19 +1964,19 @@
       <c r="C8" s="2">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>140</v>
+      <c r="E8" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>140</v>
+      <c r="B9" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1990,51 +1993,51 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>140</v>
+      <c r="B11" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>140</v>
+      <c r="B12" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>140</v>
+      <c r="B13" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:6">

</xml_diff>

<commit_message>
BOM updates - add IF synth, filters, mixer
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F9ED97-05DE-4F88-8B05-8D499F396748}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E4DAC8-6A68-4ABE-AE05-966DA004F4CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="2940" yWindow="1390" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Boards" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boards!$A$5:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boards!$A$5:$H$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="162">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -501,6 +501,27 @@
   </si>
   <si>
     <t>diplexer-GPS-RF360-B8666</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>test-boards</t>
+  </si>
+  <si>
+    <t>BOM File</t>
+  </si>
+  <si>
+    <t>synthesizers</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>filter-misc</t>
   </si>
 </sst>
 </file>
@@ -564,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -604,6 +625,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -924,7 +948,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1020,7 +1044,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>9</v>
@@ -1708,7 +1732,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>9</v>
@@ -1906,7 +1930,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7200ED79-E8BF-4B26-BED8-4868A9C7408E}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
@@ -1918,16 +1942,18 @@
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="4" width="10.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.453125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:8" ht="13">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="13">
+    <row r="5" spans="1:8" ht="13">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
@@ -1944,26 +1970,31 @@
         <v>144</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>130</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>131</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>138</v>
@@ -1974,10 +2005,12 @@
       <c r="E7" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>138</v>
@@ -1988,169 +2021,264 @@
       <c r="E8" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>146</v>
+        <v>132</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B15" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="F15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>148</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B16" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="F16" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>134</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B17" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E17" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="F17" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B18" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E18" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
         <v>136</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E19" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B20" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E20" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="F20" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>137</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B21" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C21" s="2">
         <v>2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E21" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="F21" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:F15" xr:uid="{50C1A60C-E47A-486F-B8CF-18CEB4A5343D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F16">
+  <autoFilter ref="A5:H15" xr:uid="{50C1A60C-E47A-486F-B8CF-18CEB4A5343D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:H21">
       <sortCondition ref="A5:A15"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:H14">
     <sortCondition ref="A5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Inventory - add power boms
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E4DAC8-6A68-4ABE-AE05-966DA004F4CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD57A17E-3488-4C4A-802A-769A7E00CD09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1390" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="2770" yWindow="1670" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="163">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -473,9 +473,6 @@
     <t>Stencil</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>ORDR</t>
   </si>
   <si>
@@ -522,6 +519,12 @@
   </si>
   <si>
     <t>filter-misc</t>
+  </si>
+  <si>
+    <t>SHPED</t>
+  </si>
+  <si>
+    <t>Variations: 3.3V fix, 2.7V adj</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
       <name val="Sans"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,8 +566,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -581,11 +590,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -628,6 +646,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -948,7 +972,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1944,7 +1968,7 @@
     <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.36328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="19.7265625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.453125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13">
@@ -1970,10 +1994,10 @@
         <v>144</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>8</v>
@@ -1981,13 +2005,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2045,85 +2069,85 @@
         <v>133</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>138</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>138</v>
@@ -2134,98 +2158,99 @@
       <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="E15" s="19"/>
       <c r="F15" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="E16" s="19"/>
       <c r="F16" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>134</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>138</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>146</v>
+      <c r="B18" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="17"/>
+      <c r="F18" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G18" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>159</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>136</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>146</v>
+      <c r="B19" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>138</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>143</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>138</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -2242,33 +2267,33 @@
         <v>138</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
     </row>

</xml_diff>

<commit_message>
Inventory - add pwr brd bom variations, add LNA boms, update board inv.
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD57A17E-3488-4C4A-802A-769A7E00CD09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786553C4-D3D1-4269-9C6F-295B04515FA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2770" yWindow="1670" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="1600" yWindow="1350" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -473,9 +473,6 @@
     <t>Stencil</t>
   </si>
   <si>
-    <t>ORDR</t>
-  </si>
-  <si>
     <t>microstrip-test-4-layer-sma-34-40</t>
   </si>
   <si>
@@ -503,9 +500,6 @@
     <t>BOM</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>test-boards</t>
   </si>
   <si>
@@ -524,7 +518,29 @@
     <t>SHPED</t>
   </si>
   <si>
-    <t>Variations: 3.3V fix, 2.7V adj</t>
+    <t>amps</t>
+  </si>
+  <si>
+    <t>CART</t>
+  </si>
+  <si>
+    <t>amp-LNA-BFP740Fxxx</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Variations: 3.3V fix, 2.7V adj, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Sans"/>
+      </rPr>
+      <t>5.0V fix (cart)</t>
+    </r>
+  </si>
+  <si>
+    <t>Variations: 3.3V fix</t>
   </si>
 </sst>
 </file>
@@ -534,7 +550,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -546,8 +562,13 @@
       <color rgb="FF000000"/>
       <name val="Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Sans"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,6 +590,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,9 +669,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -652,6 +676,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -972,7 +999,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33:G33"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1957,7 +1984,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1966,9 +1993,9 @@
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="4" width="10.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.08984375" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13">
@@ -1994,10 +2021,10 @@
         <v>144</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>8</v>
@@ -2005,16 +2032,20 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="E6" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -2029,8 +2060,12 @@
       <c r="E7" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="F7" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -2045,8 +2080,12 @@
       <c r="E8" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="F8" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -2061,93 +2100,99 @@
       <c r="E9" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>145</v>
+      <c r="B10" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>160</v>
+      <c r="F10" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>160</v>
+      <c r="B11" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17" t="s">
-        <v>160</v>
+        <v>150</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17" t="s">
-        <v>160</v>
+        <v>151</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>138</v>
@@ -2158,96 +2203,101 @@
       <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="E15" s="19"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>156</v>
+        <v>138</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E16" s="19"/>
+        <v>146</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="18"/>
       <c r="F16" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>156</v>
+        <v>138</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>145</v>
+      <c r="B17" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>160</v>
+      <c r="F17" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>161</v>
+      <c r="B18" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="17" t="s">
+      <c r="F18" s="17" t="s">
         <v>159</v>
       </c>
+      <c r="G18" s="16" t="s">
+        <v>157</v>
+      </c>
       <c r="H18" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>136</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>161</v>
+      <c r="B19" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17" t="s">
-        <v>159</v>
+      <c r="F19" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>143</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>145</v>
+      <c r="B20" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>158</v>
+      <c r="F20" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2267,35 +2317,38 @@
         <v>138</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>158</v>
+        <v>138</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:H15" xr:uid="{50C1A60C-E47A-486F-B8CF-18CEB4A5343D}">

</xml_diff>

<commit_message>
Update inventory and BOMs for parts received and add TPS62112 bom
</commit_message>
<xml_diff>
--- a/bom/inventory.xlsx
+++ b/bom/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786553C4-D3D1-4269-9C6F-295B04515FA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639D5C48-EC18-4BC6-AA83-B1145827CAD0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1350" windowWidth="24000" windowHeight="12760" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
+    <workbookView xWindow="1360" yWindow="530" windowWidth="25580" windowHeight="15470" activeTab="1" xr2:uid="{89C19F82-CB44-4DB1-A809-9A6D12CA2984}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boards!$A$5:$H$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$4:$H$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="220">
   <si>
     <t>Inventory of parts for all boards</t>
   </si>
@@ -173,12 +173,6 @@
     <t>634-SI4123-D-GM</t>
   </si>
   <si>
-    <t>Revision History</t>
-  </si>
-  <si>
-    <t>Rev</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -515,32 +509,193 @@
     <t>filter-misc</t>
   </si>
   <si>
+    <t>amps</t>
+  </si>
+  <si>
+    <t>amp-LNA-BFP740Fxxx</t>
+  </si>
+  <si>
+    <t>BAS16XV2T1G</t>
+  </si>
+  <si>
+    <t>Diode, Gen Purp, 200mA, SOD523</t>
+  </si>
+  <si>
+    <t>BAS16XV2T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>CL31A226KOHNNNE</t>
+  </si>
+  <si>
+    <t>C - 1206, 22u, X5R, 16V</t>
+  </si>
+  <si>
+    <t>1276-3048-1-ND</t>
+  </si>
+  <si>
+    <t>LP38692MP-ADJ/NOPB</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulator, 1A, EN, Adjustable</t>
+  </si>
+  <si>
+    <t>LP38692MP-ADJ/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>DMP2120U-7</t>
+  </si>
+  <si>
+    <t>MOSFET, P-Chan, 20V, SOT23</t>
+  </si>
+  <si>
+    <t>DMP2120U-7DICT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT1K50‎</t>
+  </si>
+  <si>
+    <t>R - 0603, 1.5k, 1%, 100ppm</t>
+  </si>
+  <si>
+    <t>‎RMCF0603FT1K50CT-ND</t>
+  </si>
+  <si>
+    <t>Susumu</t>
+  </si>
+  <si>
+    <t>PAT1220-C-2DB-T5</t>
+  </si>
+  <si>
+    <t>AT, 0805, 100mW, 2dB</t>
+  </si>
+  <si>
+    <t>PAT122CT-ND</t>
+  </si>
+  <si>
+    <t>PAT1220-C-4DB-T5</t>
+  </si>
+  <si>
+    <t>AT, 0805, 100mW, 4dB</t>
+  </si>
+  <si>
+    <t>PAT124CT-ND</t>
+  </si>
+  <si>
+    <t>PAT1220-C-6DB-T5</t>
+  </si>
+  <si>
+    <t>AT, 0805, 100mW, 6dB</t>
+  </si>
+  <si>
+    <t>PAT126CT-ND</t>
+  </si>
+  <si>
+    <t>PAT1220-C-8DB-T5</t>
+  </si>
+  <si>
+    <t>AT, 0805, 100mW, 8dB</t>
+  </si>
+  <si>
+    <t>PAT128CT-ND</t>
+  </si>
+  <si>
+    <t>AVX Corp</t>
+  </si>
+  <si>
+    <t>BP0805A1308ASTR</t>
+  </si>
+  <si>
+    <t>Filter, thin-film 0805, 1220 - 1420 MHz</t>
+  </si>
+  <si>
+    <t>478-12187-1-ND</t>
+  </si>
+  <si>
+    <t>RF360</t>
+  </si>
+  <si>
+    <t>B39162B8666L210</t>
+  </si>
+  <si>
+    <t>Diplexer, GPS SAW extractor</t>
+  </si>
+  <si>
+    <t>B39162B8666L210CT-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RT0402BRD0711K8L‎</t>
+  </si>
+  <si>
+    <t>R - 0402, 11.8k, 0.1%, 25ppm</t>
+  </si>
+  <si>
+    <t>‎YAG4166CT-ND‎</t>
+  </si>
+  <si>
+    <t>RT0402BRD0713K7L‎</t>
+  </si>
+  <si>
+    <t>R - 0402, 13.7k, 0.1%, 25ppm</t>
+  </si>
+  <si>
+    <t>‎YAG4172CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT5K60</t>
+  </si>
+  <si>
+    <t>R - 0603, 5.6k, 1%, 100ppm</t>
+  </si>
+  <si>
+    <t>RMCF0603FT5K60CT-ND</t>
+  </si>
+  <si>
+    <t>M20-9980645</t>
+  </si>
+  <si>
+    <t>2.54mm header, vertical strip, 12 pos (2x6)</t>
+  </si>
+  <si>
+    <t>952-2125-ND</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Assembled 1x mixer-MAC-24+ w/ all 0 ohm</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
     <t>SHPED</t>
   </si>
   <si>
-    <t>amps</t>
-  </si>
-  <si>
-    <t>CART</t>
-  </si>
-  <si>
-    <t>amp-LNA-BFP740Fxxx</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Variations: 3.3V fix, 2.7V adj, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Sans"/>
-      </rPr>
-      <t>5.0V fix (cart)</t>
-    </r>
-  </si>
-  <si>
-    <t>Variations: 3.3V fix</t>
+    <t>Used for L and S band</t>
+  </si>
+  <si>
+    <t>Variations: 3.3V fix, 5.0V fix (shped)</t>
+  </si>
+  <si>
+    <t>Variations: 3.3V fix, 2.7V adj, 5.0V fix (shped)</t>
+  </si>
+  <si>
+    <t>REORD</t>
+  </si>
+  <si>
+    <t>Redesign stencil for fixed tCream mixer</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Board</t>
   </si>
 </sst>
 </file>
@@ -564,7 +719,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Sans"/>
     </font>
   </fonts>
@@ -589,18 +743,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -617,20 +771,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color auto="1"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -675,10 +820,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -995,16 +1150,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C355E92D-4F29-4448-8517-BC8F08AC5F2B}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
@@ -1047,381 +1202,383 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>208</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2">
-        <v>98</v>
+        <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>177</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>179</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>180</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>185</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>186</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6"/>
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="6"/>
+      <c r="C14" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="6"/>
+      <c r="C15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="C16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>53</v>
+      <c r="C17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>90</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>55</v>
+      <c r="C18" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>164</v>
       </c>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>59</v>
+      <c r="C20" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>161</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -1433,73 +1590,69 @@
         <v>9</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>194</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" t="s">
-        <v>99</v>
-      </c>
+      <c r="C22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
-        <v>101</v>
-      </c>
+      <c r="C23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
@@ -1508,252 +1661,258 @@
         <v>32</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>22</v>
+      <c r="C25" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>191</v>
       </c>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>24</v>
+      <c r="A29" s="2">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="E31" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2">
+        <v>9</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2">
+        <v>9</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" t="s">
-        <v>78</v>
-      </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" t="s">
-        <v>141</v>
+      <c r="C34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="H34" s="6"/>
     </row>
@@ -1765,143 +1924,424 @@
         <v>9</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>71</v>
-      </c>
+      <c r="C36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="2">
+        <v>3</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="2">
+        <v>4</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="2">
+        <v>19</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="2">
+        <v>3</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" t="s">
+        <v>198</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="2">
+        <v>3</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" t="s">
+        <v>200</v>
+      </c>
+      <c r="E43" t="s">
+        <v>201</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>202</v>
+      </c>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="2">
+        <v>96</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="2">
+        <v>92</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="2">
+        <v>10</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" t="s">
+        <v>173</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2">
+        <v>98</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="2">
+        <v>10</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" t="s">
+        <v>203</v>
+      </c>
+      <c r="E48" t="s">
+        <v>204</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" t="s">
+        <v>205</v>
+      </c>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="2">
+        <v>10</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="2">
+        <v>1</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="2">
+        <v>94</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" t="s">
+        <v>69</v>
+      </c>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="2">
+        <v>9</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G52" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="B38" s="8"/>
-      <c r="C38" s="13"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="B39" s="8"/>
-      <c r="C39" s="13"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="B40" s="8"/>
-      <c r="C40" s="13"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="B41" s="8"/>
-      <c r="C41" s="13"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="B42" s="8"/>
-      <c r="C42" s="13"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="B43" s="8"/>
-      <c r="C43" s="13"/>
-      <c r="H43" s="6"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="B44" s="8"/>
-      <c r="C44" s="13"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="B45" s="8"/>
-      <c r="C45" s="13"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="B46" s="8"/>
-      <c r="C46" s="13"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="B47" s="8"/>
-      <c r="C47" s="13"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="B48" s="8"/>
-      <c r="C48" s="13"/>
-      <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="B49" s="8"/>
-      <c r="C49" s="13"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="B50" s="8"/>
-      <c r="C50" s="13"/>
-      <c r="H50" s="6"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="B51" s="8"/>
-      <c r="C51" s="13"/>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="B52" s="8"/>
-      <c r="C52" s="13"/>
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8">
@@ -1910,68 +2350,111 @@
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="57" spans="1:8" ht="13">
-      <c r="A57" s="1" t="s">
+      <c r="B54" s="8"/>
+      <c r="C54" s="13"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="B55" s="8"/>
+      <c r="C55" s="13"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" s="8"/>
+      <c r="C56" s="13"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" s="8"/>
+      <c r="C57" s="13"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="B58" s="8"/>
+      <c r="C58" s="13"/>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" s="8"/>
+      <c r="C59" s="13"/>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" s="8"/>
+      <c r="C60" s="13"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="B61" s="8"/>
+      <c r="C61" s="13"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" s="8"/>
+      <c r="C62" s="13"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="66" spans="1:4" ht="13">
+      <c r="A66" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="13">
+      <c r="A68" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="2" t="s">
+      <c r="B68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B69" t="s">
         <v>47</v>
       </c>
-      <c r="C59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="2">
-        <v>1</v>
-      </c>
-      <c r="B60" s="2" t="s">
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="12">
+        <v>43675</v>
+      </c>
+      <c r="B70" t="s">
         <v>48</v>
       </c>
-      <c r="C60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="2">
-        <v>2</v>
-      </c>
-      <c r="B61" s="12">
-        <v>43675</v>
-      </c>
-      <c r="C61" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="2">
-        <v>3</v>
-      </c>
-      <c r="B62" s="12">
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="12">
         <v>43700</v>
       </c>
-      <c r="C62" t="s">
-        <v>102</v>
+      <c r="B71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="12">
+        <v>43738</v>
+      </c>
+      <c r="B72" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H54" xr:uid="{12ABAAD2-10AD-445B-A38F-77CAAD4446E7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H54">
-      <sortCondition ref="E4:E54"/>
+  <autoFilter ref="A4:H63" xr:uid="{12ABAAD2-10AD-445B-A38F-77CAAD4446E7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H63">
+      <sortCondition ref="E4:E63"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1984,47 +2467,44 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="30.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10" style="2" customWidth="1"/>
-    <col min="3" max="4" width="10.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="2" customWidth="1"/>
+    <col min="2" max="6" width="11.1796875" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.7265625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="36.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.90625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" s="14"/>
     </row>
     <row r="5" spans="1:8" ht="13">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>219</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>8</v>
@@ -2032,303 +2512,337 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>161</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>161</v>
+        <v>145</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>161</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="16"/>
+        <v>136</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>212</v>
+      </c>
       <c r="G9" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>159</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>159</v>
+        <v>131</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>159</v>
+        <v>147</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>159</v>
+      <c r="B13" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>159</v>
+        <v>149</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>2</v>
-      </c>
-      <c r="E15" s="18"/>
+        <v>150</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>146</v>
+      </c>
       <c r="F15" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="18"/>
+        <v>136</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>218</v>
+      </c>
       <c r="F16" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>159</v>
+        <v>136</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>159</v>
+        <v>136</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>161</v>
+        <v>136</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>164</v>
+        <v>155</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>159</v>
+        <v>136</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21" s="2">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>162</v>
-      </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+        <v>135</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="F23" s="16"/>
@@ -2352,7 +2866,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A5:H15" xr:uid="{50C1A60C-E47A-486F-B8CF-18CEB4A5343D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:H21">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:H22">
       <sortCondition ref="A5:A15"/>
     </sortState>
   </autoFilter>

</xml_diff>